<commit_message>
Diagrama de classe e especificação de classe
Diagrama de classe e especificação de classe
</commit_message>
<xml_diff>
--- a/docs/tabelas.xlsx
+++ b/docs/tabelas.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documentos\GitHub\osm\odonto-system-manager\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\Documents\GitHub\odonto-system-manager\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7680"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7680" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Gerenciamento de riscos" sheetId="1" r:id="rId1"/>
     <sheet name="Cronograma" sheetId="2" r:id="rId2"/>
+    <sheet name="Diagrama de classe" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="144">
   <si>
     <t>Mudança de requisitos</t>
   </si>
@@ -235,13 +237,580 @@
   </si>
   <si>
     <t>10 dias</t>
+  </si>
+  <si>
+    <t>Métodos</t>
+  </si>
+  <si>
+    <t>cadastrarUsuario</t>
+  </si>
+  <si>
+    <t>editarUsuario</t>
+  </si>
+  <si>
+    <t>adicionarPermissao</t>
+  </si>
+  <si>
+    <t>editarAnamnese</t>
+  </si>
+  <si>
+    <t>Edita cadastro de usuário</t>
+  </si>
+  <si>
+    <t>Cadastra novo usuário</t>
+  </si>
+  <si>
+    <t>Inativa o cadastro de usuário</t>
+  </si>
+  <si>
+    <t>Adiciona permissões a um usuário</t>
+  </si>
+  <si>
+    <t>Revogar permissões a um usuário</t>
+  </si>
+  <si>
+    <t>Edita anamnese de um usuário</t>
+  </si>
+  <si>
+    <t>inativarUsuario</t>
+  </si>
+  <si>
+    <t>revogarPermissao</t>
+  </si>
+  <si>
+    <t>editarDescricao</t>
+  </si>
+  <si>
+    <t>Edita descrição de uma permissão</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Classe: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Permissão</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Classe destinada a manter as permissões do sistema</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Classe: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Usuario</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Classe destinada a manter usuários do sistema</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Classe: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Login</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Classe destinada a realizar operações de login no sistema</t>
+    </r>
+  </si>
+  <si>
+    <t>realizarLogin</t>
+  </si>
+  <si>
+    <t>verificarExistenciaUsuario</t>
+  </si>
+  <si>
+    <t>iniciarSessao</t>
+  </si>
+  <si>
+    <t>redirecionarUsuario</t>
+  </si>
+  <si>
+    <t>terminarSessao</t>
+  </si>
+  <si>
+    <t>validarLogin</t>
+  </si>
+  <si>
+    <t>Efetua login no sistema</t>
+  </si>
+  <si>
+    <t>Verifica existencia de usuário previamente cadastrado</t>
+  </si>
+  <si>
+    <t>Valida login no sistema</t>
+  </si>
+  <si>
+    <t>Inicia sessão no sistema</t>
+  </si>
+  <si>
+    <t>Redireciona usuário para pagina inicial</t>
+  </si>
+  <si>
+    <t>Termina sessão do sistema, realizando logout do usuario</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Classe: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Entidade</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - DESCREVER</t>
+    </r>
+  </si>
+  <si>
+    <t>Atributos</t>
+  </si>
+  <si>
+    <t>ativo</t>
+  </si>
+  <si>
+    <t>isAtivo</t>
+  </si>
+  <si>
+    <t>inativar</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Classe: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Resposta</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - DESCREVER</t>
+    </r>
+  </si>
+  <si>
+    <t>respostaTexto</t>
+  </si>
+  <si>
+    <t>respostaBool</t>
+  </si>
+  <si>
+    <t>outro</t>
+  </si>
+  <si>
+    <t>editarTipo</t>
+  </si>
+  <si>
+    <t>adicionarPergunta</t>
+  </si>
+  <si>
+    <t>adicionarResposta</t>
+  </si>
+  <si>
+    <t>adicionarRespostaOpcional</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Classe: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Anamnese</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - DESCREVER</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Classe: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Pergunta</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - DESCREVER</t>
+    </r>
+  </si>
+  <si>
+    <t>editarPergunta</t>
+  </si>
+  <si>
+    <t>novaPergunta</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Classe: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Material</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - DESCREVER</t>
+    </r>
+  </si>
+  <si>
+    <t>adicionarEntrada</t>
+  </si>
+  <si>
+    <t>removerQuantidade</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Classe: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>MaterialEstoque</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - DESCREVER</t>
+    </r>
+  </si>
+  <si>
+    <t>material</t>
+  </si>
+  <si>
+    <t>quantidade</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Classe: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>AcaoServico_has_Material</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - DESCREVER</t>
+    </r>
+  </si>
+  <si>
+    <t>adicionarQuantidade</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Classe: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>AcaoServico</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - DESCREVER</t>
+    </r>
+  </si>
+  <si>
+    <t>servico</t>
+  </si>
+  <si>
+    <t>adicionarMaterial</t>
+  </si>
+  <si>
+    <t>alterarPreco</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Classe: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Servico</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - DESCREVER</t>
+    </r>
+  </si>
+  <si>
+    <t>novoServico</t>
+  </si>
+  <si>
+    <t>remover</t>
+  </si>
+  <si>
+    <t>editarNome</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Classe: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Atendimento</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - DESCREVER</t>
+    </r>
+  </si>
+  <si>
+    <t>adicionarServico</t>
+  </si>
+  <si>
+    <t>finalizar</t>
+  </si>
+  <si>
+    <t>removerServico</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Classe: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Agendamento</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - DESCREVER</t>
+    </r>
+  </si>
+  <si>
+    <t>iniciarAtendimento</t>
+  </si>
+  <si>
+    <t>gerarMulta</t>
+  </si>
+  <si>
+    <t>cancelarAgendamento</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Classe: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>AgendaOdontologo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - DESCREVER</t>
+    </r>
+  </si>
+  <si>
+    <t>adicionarAgendamento</t>
+  </si>
+  <si>
+    <t>removerAgendamento</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -249,8 +818,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -269,8 +846,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -278,11 +861,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -300,12 +898,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -317,6 +909,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -634,96 +1244,96 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.140625" style="11"/>
-    <col min="2" max="2" width="38.28515625" style="11" customWidth="1"/>
-    <col min="3" max="16384" width="30.140625" style="11"/>
+    <col min="1" max="1" width="30.140625" style="9"/>
+    <col min="2" max="2" width="38.28515625" style="9" customWidth="1"/>
+    <col min="3" max="16384" width="30.140625" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="9" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="12">
+      <c r="C2" s="10">
         <v>0.3</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="10">
         <v>0.4</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="10">
         <v>0.6</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="10">
         <v>0.25</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="10">
         <v>0.25</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="10">
         <v>0.3</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C8" s="13"/>
+      <c r="C8" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -758,11 +1368,11 @@
       <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
       <c r="D2" s="5" t="s">
         <v>52</v>
       </c>
@@ -772,10 +1382,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="9"/>
+      <c r="C3" s="16"/>
       <c r="D3" s="5" t="s">
         <v>63</v>
       </c>
@@ -783,10 +1393,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="9"/>
+      <c r="C4" s="16"/>
       <c r="D4" s="8" t="s">
         <v>63</v>
       </c>
@@ -794,10 +1404,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="9"/>
+      <c r="C5" s="16"/>
       <c r="D5" s="8" t="s">
         <v>63</v>
       </c>
@@ -805,10 +1415,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="9"/>
+      <c r="C6" s="16"/>
       <c r="D6" s="5" t="s">
         <v>53</v>
       </c>
@@ -838,11 +1448,11 @@
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
       <c r="D9" s="6" t="s">
         <v>51</v>
       </c>
@@ -852,10 +1462,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="10"/>
+      <c r="C10" s="17"/>
       <c r="D10" s="6" t="s">
         <v>53</v>
       </c>
@@ -896,10 +1506,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="10"/>
+      <c r="C14" s="17"/>
       <c r="D14" s="6" t="s">
         <v>68</v>
       </c>
@@ -928,11 +1538,11 @@
       <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
       <c r="D17" s="5" t="s">
         <v>53</v>
       </c>
@@ -942,10 +1552,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="9"/>
+      <c r="C18" s="16"/>
       <c r="D18" s="5" t="s">
         <v>64</v>
       </c>
@@ -953,10 +1563,10 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="9"/>
+      <c r="C19" s="16"/>
       <c r="D19" s="5" t="s">
         <v>57</v>
       </c>
@@ -975,10 +1585,10 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="9"/>
+      <c r="C21" s="16"/>
       <c r="D21" s="8" t="s">
         <v>64</v>
       </c>
@@ -986,21 +1596,21 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="9"/>
+      <c r="C22" s="16"/>
       <c r="D22" s="8" t="s">
         <v>57</v>
       </c>
       <c r="E22" s="4"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
       <c r="D23" s="6" t="s">
         <v>54</v>
       </c>
@@ -1010,10 +1620,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="10"/>
+      <c r="C24" s="17"/>
       <c r="D24" s="6" t="s">
         <v>64</v>
       </c>
@@ -1021,10 +1631,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="10"/>
+      <c r="C25" s="17"/>
       <c r="D25" s="6">
         <v>15</v>
       </c>
@@ -1064,11 +1674,11 @@
       <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
+      <c r="A29" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="16"/>
       <c r="D29" s="5" t="s">
         <v>54</v>
       </c>
@@ -1078,10 +1688,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
-      <c r="B30" s="9" t="s">
+      <c r="B30" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="9"/>
+      <c r="C30" s="16"/>
       <c r="D30" s="8" t="s">
         <v>57</v>
       </c>
@@ -1089,10 +1699,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
-      <c r="B31" s="9" t="s">
+      <c r="B31" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="C31" s="9"/>
+      <c r="C31" s="16"/>
       <c r="D31" s="5" t="s">
         <v>53</v>
       </c>
@@ -1100,10 +1710,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="C32" s="9"/>
+      <c r="C32" s="16"/>
       <c r="D32" s="5" t="s">
         <v>67</v>
       </c>
@@ -1218,4 +1828,584 @@
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B94"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="A95" sqref="A95"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.5703125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="33.140625" style="9" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="18"/>
+    </row>
+    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" s="14"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5" s="14"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="B6" s="14"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" s="18"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="B17" s="18"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="B21" s="18"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="B30" s="18"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="B32" s="14"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="B33" s="14"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="B34" s="14"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="B35" s="14"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="B37" s="18"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="B39" s="14"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="B40" s="14"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="B41" s="14"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="B43" s="14"/>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="B45" s="18"/>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B46" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="B47" s="14"/>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="B48" s="14"/>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="B50" s="18"/>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B51" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="B52" s="14"/>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="B53" s="14"/>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="B55" s="18"/>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B56" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="B57" s="14"/>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="B58" s="14"/>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="B60" s="18"/>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B61" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="B62" s="14"/>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="B64" s="18"/>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B65" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="B66" s="14"/>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B67" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="B68" s="14"/>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B69" s="14"/>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="B71" s="18"/>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B72" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="B73" s="14"/>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="B74" s="14"/>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="B75" s="14"/>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="B76" s="14"/>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="B77" s="14"/>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="B79" s="18"/>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B80" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="B81" s="14"/>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="B82" s="14"/>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="B83" s="14"/>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="B85" s="18"/>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B86" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="B87" s="14"/>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="B88" s="14"/>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="B89" s="14"/>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="B91" s="18"/>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B92" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="B93" s="14"/>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="B94" s="14"/>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A30:B30"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>